<commit_message>
Fix tickers table creation command and update table structure files
</commit_message>
<xml_diff>
--- a/table_structure.xlsx
+++ b/table_structure.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="215">
   <si>
     <t xml:space="preserve">baskets</t>
   </si>
@@ -310,10 +310,10 @@
     <t xml:space="preserve">ticker</t>
   </si>
   <si>
-    <t xml:space="preserve">exchanges(abbrev)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">child_exchange</t>
+    <t xml:space="preserve">INT NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exchanges(exchange_id)</t>
   </si>
   <si>
     <t xml:space="preserve">sector</t>
@@ -766,18 +766,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D341"/>
+  <dimension ref="A1:D340"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A87" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C124" activeCellId="0" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8785425101215"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.9352226720648"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.3076923076923"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.1902834008097"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.7935222672065"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.2793522267206"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1779,31 +1779,31 @@
         <v>40</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>97</v>
+        <v>42</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B126" s="0" t="s">
         <v>12</v>
@@ -1811,34 +1811,34 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B128" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="D128" s="0" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B129" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="D129" s="0" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B130" s="0" t="s">
         <v>10</v>
@@ -1846,7 +1846,7 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="B131" s="0" t="s">
         <v>10</v>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>65</v>
+        <v>102</v>
       </c>
       <c r="B132" s="0" t="s">
         <v>10</v>
@@ -1862,83 +1862,86 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="C133" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C134" s="0" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B135" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B136" s="0" t="s">
-        <v>12</v>
+    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>103</v>
+        <v>1</v>
+      </c>
+      <c r="B138" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C138" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D138" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>1</v>
+        <v>104</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C139" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D139" s="0" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>19</v>
+        <v>43</v>
+      </c>
+      <c r="C140" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D140" s="0" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D141" s="0" t="s">
-        <v>107</v>
+        <v>23</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B142" s="0" t="s">
         <v>8</v>
@@ -1946,16 +1949,16 @@
       <c r="C142" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="D142" s="0" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C143" s="0" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="D143" s="0" t="s">
         <v>107</v>
@@ -1963,18 +1966,15 @@
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D144" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>69</v>
+        <v>111</v>
       </c>
       <c r="B145" s="0" t="s">
         <v>110</v>
@@ -1982,7 +1982,7 @@
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B146" s="0" t="s">
         <v>110</v>
@@ -1990,7 +1990,7 @@
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>112</v>
+        <v>70</v>
       </c>
       <c r="B147" s="0" t="s">
         <v>110</v>
@@ -1998,77 +1998,80 @@
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>70</v>
+        <v>113</v>
       </c>
       <c r="B148" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>117</v>
+        <v>16</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B152" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D152" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D151" s="0" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>118</v>
+        <v>1</v>
+      </c>
+      <c r="B154" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C154" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D154" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>1</v>
+        <v>119</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C155" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D155" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>119</v>
+        <v>22</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="C156" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B157" s="0" t="s">
         <v>8</v>
@@ -2076,32 +2079,29 @@
       <c r="C157" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="D157" s="0" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="B158" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C158" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D158" s="0" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>109</v>
+        <v>30</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B160" s="0" t="s">
         <v>30</v>
@@ -2109,7 +2109,7 @@
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B161" s="0" t="s">
         <v>30</v>
@@ -2117,64 +2117,70 @@
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>123</v>
+        <v>16</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B163" s="0" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>124</v>
+        <v>1</v>
+      </c>
+      <c r="B165" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C165" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D165" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="B166" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C166" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D166" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>125</v>
+        <v>49</v>
       </c>
       <c r="B167" s="0" t="s">
-        <v>19</v>
+        <v>43</v>
+      </c>
+      <c r="C167" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D167" s="0" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>106</v>
+        <v>23</v>
       </c>
       <c r="D168" s="0" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B169" s="0" t="s">
         <v>8</v>
@@ -2186,15 +2192,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C170" s="0" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="D170" s="0" t="s">
         <v>126</v>
@@ -2202,99 +2205,99 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="B171" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D171" s="0" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B172" s="0" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B173" s="0" t="s">
-        <v>129</v>
+        <v>10</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>130</v>
+        <v>15</v>
       </c>
       <c r="B174" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B175" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B176" s="0" t="s">
-        <v>12</v>
+    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>131</v>
+        <v>1</v>
+      </c>
+      <c r="B178" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C178" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D178" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="B179" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C179" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D179" s="0" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>132</v>
+        <v>49</v>
       </c>
       <c r="B180" s="0" t="s">
-        <v>19</v>
+        <v>43</v>
+      </c>
+      <c r="C180" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D180" s="0" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B181" s="0" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C181" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D181" s="0" t="s">
-        <v>133</v>
+        <v>23</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B182" s="0" t="s">
         <v>8</v>
@@ -2302,16 +2305,16 @@
       <c r="C182" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="D182" s="0" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C183" s="0" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D183" s="0" t="s">
         <v>133</v>
@@ -2319,18 +2322,15 @@
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="B184" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D184" s="0" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="B185" s="0" t="s">
         <v>110</v>
@@ -2338,7 +2338,7 @@
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B186" s="0" t="s">
         <v>110</v>
@@ -2346,7 +2346,7 @@
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
       <c r="B187" s="0" t="s">
         <v>110</v>
@@ -2354,67 +2354,73 @@
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>69</v>
+        <v>113</v>
       </c>
       <c r="B188" s="0" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="B189" s="0" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="B190" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D190" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D189" s="0" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>136</v>
+        <v>1</v>
+      </c>
+      <c r="B192" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C192" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D192" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>1</v>
+        <v>137</v>
       </c>
       <c r="B193" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C193" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D193" s="0" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>137</v>
+        <v>49</v>
       </c>
       <c r="B194" s="0" t="s">
-        <v>19</v>
+        <v>43</v>
+      </c>
+      <c r="C194" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D194" s="0" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B195" s="0" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C195" s="0" t="s">
-        <v>106</v>
+        <v>23</v>
       </c>
       <c r="D195" s="0" t="s">
         <v>138</v>
@@ -2422,7 +2428,7 @@
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B196" s="0" t="s">
         <v>8</v>
@@ -2436,21 +2442,15 @@
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B197" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C197" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D197" s="0" t="s">
-        <v>138</v>
+        <v>10</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B198" s="0" t="s">
         <v>10</v>
@@ -2458,7 +2458,7 @@
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="B199" s="0" t="s">
         <v>10</v>
@@ -2466,26 +2466,29 @@
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>65</v>
+        <v>139</v>
       </c>
       <c r="B200" s="0" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B201" s="0" t="s">
-        <v>43</v>
+        <v>90</v>
+      </c>
+      <c r="D201" s="0" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B202" s="0" t="s">
-        <v>90</v>
+        <v>44</v>
       </c>
       <c r="D202" s="0" t="s">
         <v>138</v>
@@ -2493,29 +2496,29 @@
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>141</v>
+        <v>92</v>
       </c>
       <c r="B203" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="D203" s="0" t="s">
-        <v>138</v>
+        <v>10</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>92</v>
+        <v>142</v>
       </c>
       <c r="B204" s="0" t="s">
-        <v>10</v>
+        <v>143</v>
+      </c>
+      <c r="D204" s="0" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D205" s="0" t="s">
         <v>138</v>
@@ -2523,67 +2526,70 @@
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>144</v>
+        <v>15</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="D206" s="0" t="s">
-        <v>138</v>
+        <v>12</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B207" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B208" s="0" t="s">
-        <v>12</v>
+    <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>146</v>
+        <v>1</v>
+      </c>
+      <c r="B210" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C210" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D210" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>1</v>
+        <v>147</v>
       </c>
       <c r="B211" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C211" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D211" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>147</v>
+        <v>49</v>
       </c>
       <c r="B212" s="0" t="s">
-        <v>19</v>
+        <v>43</v>
+      </c>
+      <c r="C212" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D212" s="0" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>49</v>
+        <v>137</v>
       </c>
       <c r="B213" s="0" t="s">
-        <v>43</v>
+        <v>114</v>
       </c>
       <c r="C213" s="0" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="D213" s="0" t="s">
         <v>148</v>
@@ -2591,72 +2597,66 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="B214" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="C214" s="0" t="s">
-        <v>149</v>
+        <v>12</v>
       </c>
       <c r="D214" s="0" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="B215" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D215" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B216" s="0" t="s">
-        <v>151</v>
+        <v>30</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B217" s="0" t="s">
-        <v>30</v>
+        <v>151</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B218" s="0" t="s">
-        <v>151</v>
+        <v>30</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>154</v>
+        <v>70</v>
       </c>
       <c r="B219" s="0" t="s">
-        <v>30</v>
+        <v>151</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>70</v>
+        <v>155</v>
       </c>
       <c r="B220" s="0" t="s">
-        <v>151</v>
+        <v>30</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>155</v>
+        <v>113</v>
       </c>
       <c r="B221" s="0" t="s">
         <v>30</v>
@@ -2664,23 +2664,23 @@
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>113</v>
+        <v>156</v>
       </c>
       <c r="B222" s="0" t="s">
-        <v>30</v>
+        <v>157</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B223" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B224" s="0" t="s">
         <v>159</v>
@@ -2688,7 +2688,7 @@
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B225" s="0" t="s">
         <v>159</v>
@@ -2696,7 +2696,7 @@
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B226" s="0" t="s">
         <v>159</v>
@@ -2704,7 +2704,7 @@
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B227" s="0" t="s">
         <v>159</v>
@@ -2712,61 +2712,67 @@
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>163</v>
+        <v>16</v>
       </c>
       <c r="B228" s="0" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B229" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="1" t="s">
         <v>164</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B231" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C231" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D231" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>1</v>
+        <v>165</v>
       </c>
       <c r="B232" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C232" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D232" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="B233" s="0" t="s">
-        <v>19</v>
+        <v>43</v>
+      </c>
+      <c r="C233" s="0" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B234" s="0" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C234" s="0" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+      <c r="D234" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B235" s="0" t="s">
         <v>8</v>
@@ -2780,13 +2786,10 @@
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="B236" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C236" s="0" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D236" s="0" t="s">
         <v>166</v>
@@ -2794,18 +2797,15 @@
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="B237" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D237" s="0" t="s">
-        <v>166</v>
+        <v>110</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B238" s="0" t="s">
         <v>110</v>
@@ -2813,7 +2813,7 @@
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="B239" s="0" t="s">
         <v>110</v>
@@ -2821,7 +2821,7 @@
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>167</v>
+        <v>111</v>
       </c>
       <c r="B240" s="0" t="s">
         <v>110</v>
@@ -2829,7 +2829,7 @@
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B241" s="0" t="s">
         <v>110</v>
@@ -2837,7 +2837,7 @@
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>112</v>
+        <v>70</v>
       </c>
       <c r="B242" s="0" t="s">
         <v>110</v>
@@ -2845,15 +2845,15 @@
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="B243" s="0" t="s">
-        <v>110</v>
+        <v>30</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B244" s="0" t="s">
         <v>30</v>
@@ -2861,7 +2861,7 @@
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="B245" s="0" t="s">
         <v>30</v>
@@ -2869,61 +2869,64 @@
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>168</v>
+        <v>113</v>
       </c>
       <c r="B246" s="0" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="B247" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="1" t="s">
+    <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="1" t="s">
         <v>169</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B249" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C249" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D249" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="s">
-        <v>1</v>
+        <v>165</v>
       </c>
       <c r="B250" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C250" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D250" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="B251" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+      <c r="C251" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B252" s="0" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C252" s="0" t="s">
-        <v>106</v>
+        <v>23</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B253" s="0" t="s">
         <v>8</v>
@@ -2931,16 +2934,16 @@
       <c r="C253" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="D253" s="0" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="B254" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C254" s="0" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D254" s="0" t="s">
         <v>170</v>
@@ -2948,10 +2951,10 @@
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="0" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="B255" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D255" s="0" t="s">
         <v>170</v>
@@ -2959,53 +2962,56 @@
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B256" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D256" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="B257" s="0" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="0" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="s">
-        <v>171</v>
+        <v>1</v>
+      </c>
+      <c r="B259" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C259" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D259" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="0" t="s">
-        <v>1</v>
+        <v>172</v>
       </c>
       <c r="B260" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C260" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D260" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="s">
-        <v>172</v>
+        <v>22</v>
       </c>
       <c r="B261" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="C261" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D261" s="0" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B262" s="0" t="s">
         <v>8</v>
@@ -3017,93 +3023,93 @@
         <v>173</v>
       </c>
     </row>
-    <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B263" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C263" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D263" s="0" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="B264" s="0" t="s">
-        <v>10</v>
+        <v>109</v>
+      </c>
+      <c r="D264" s="0" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="0" t="s">
-        <v>108</v>
+        <v>174</v>
       </c>
       <c r="B265" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D265" s="0" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
-        <v>174</v>
+        <v>15</v>
       </c>
       <c r="B266" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B267" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B268" s="0" t="s">
-        <v>12</v>
+    <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="0" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="0" t="s">
-        <v>175</v>
+        <v>1</v>
+      </c>
+      <c r="B270" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C270" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D270" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="0" t="s">
-        <v>1</v>
+        <v>176</v>
       </c>
       <c r="B271" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C271" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D271" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="0" t="s">
-        <v>176</v>
+        <v>22</v>
       </c>
       <c r="B272" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="C272" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D272" s="0" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B273" s="0" t="s">
         <v>8</v>
@@ -3115,23 +3121,17 @@
         <v>177</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B274" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C274" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D274" s="0" t="s">
-        <v>177</v>
+        <v>10</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="0" t="s">
-        <v>38</v>
+        <v>178</v>
       </c>
       <c r="B275" s="0" t="s">
         <v>10</v>
@@ -3139,34 +3139,34 @@
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B276" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B277" s="0" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>109</v>
+      </c>
+      <c r="D277" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B278" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D278" s="0" t="s">
-        <v>177</v>
+        <v>12</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B279" s="0" t="s">
         <v>12</v>
@@ -3174,7 +3174,7 @@
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B280" s="0" t="s">
         <v>12</v>
@@ -3182,7 +3182,7 @@
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="0" t="s">
-        <v>183</v>
+        <v>15</v>
       </c>
       <c r="B281" s="0" t="s">
         <v>12</v>
@@ -3190,50 +3190,56 @@
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B282" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B283" s="0" t="s">
-        <v>12</v>
+    <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="0" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="0" t="s">
-        <v>184</v>
+        <v>1</v>
+      </c>
+      <c r="B285" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C285" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D285" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="s">
-        <v>1</v>
+        <v>185</v>
       </c>
       <c r="B286" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C286" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D286" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
-        <v>185</v>
+        <v>22</v>
       </c>
       <c r="B287" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="C287" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D287" s="0" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B288" s="0" t="s">
         <v>8</v>
@@ -3245,50 +3251,44 @@
         <v>186</v>
       </c>
     </row>
-    <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B289" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C289" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D289" s="0" t="s">
-        <v>186</v>
+        <v>10</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="0" t="s">
-        <v>38</v>
+        <v>187</v>
       </c>
       <c r="B290" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="0" t="s">
-        <v>187</v>
+        <v>108</v>
       </c>
       <c r="B291" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>109</v>
+      </c>
+      <c r="D291" s="0" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="0" t="s">
-        <v>108</v>
+        <v>188</v>
       </c>
       <c r="B292" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D292" s="0" t="s">
-        <v>186</v>
+        <v>116</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B293" s="0" t="s">
         <v>116</v>
@@ -3296,58 +3296,64 @@
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="0" t="s">
-        <v>189</v>
+        <v>15</v>
       </c>
       <c r="B294" s="0" t="s">
-        <v>116</v>
+        <v>12</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B295" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B296" s="0" t="s">
-        <v>12</v>
+    <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A297" s="0" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="0" t="s">
-        <v>190</v>
+        <v>1</v>
+      </c>
+      <c r="B298" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C298" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D298" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="0" t="s">
-        <v>1</v>
+        <v>191</v>
       </c>
       <c r="B299" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C299" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D299" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
-        <v>191</v>
+        <v>22</v>
       </c>
       <c r="B300" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="C300" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D300" s="0" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B301" s="0" t="s">
         <v>8</v>
@@ -3361,13 +3367,10 @@
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="0" t="s">
-        <v>24</v>
+        <v>193</v>
       </c>
       <c r="B302" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C302" s="0" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D302" s="0" t="s">
         <v>192</v>
@@ -3375,37 +3378,34 @@
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="0" t="s">
-        <v>193</v>
+        <v>108</v>
       </c>
       <c r="B303" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D303" s="0" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="0" t="s">
-        <v>108</v>
+        <v>194</v>
       </c>
       <c r="B304" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="D304" s="0" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B305" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B306" s="0" t="s">
         <v>10</v>
@@ -3413,7 +3413,7 @@
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B307" s="0" t="s">
         <v>10</v>
@@ -3421,7 +3421,7 @@
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B308" s="0" t="s">
         <v>10</v>
@@ -3429,7 +3429,7 @@
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B309" s="0" t="s">
         <v>10</v>
@@ -3437,58 +3437,64 @@
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="0" t="s">
-        <v>199</v>
+        <v>15</v>
       </c>
       <c r="B310" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B311" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A312" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B312" s="0" t="s">
-        <v>12</v>
+    <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="0" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="0" t="s">
-        <v>200</v>
+        <v>1</v>
+      </c>
+      <c r="B314" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C314" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D314" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="0" t="s">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="B315" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C315" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D315" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="0" t="s">
-        <v>201</v>
+        <v>22</v>
       </c>
       <c r="B316" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="C316" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D316" s="0" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B317" s="0" t="s">
         <v>8</v>
@@ -3500,50 +3506,44 @@
         <v>202</v>
       </c>
     </row>
-    <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B318" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C318" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D318" s="0" t="s">
-        <v>202</v>
+        <v>10</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="0" t="s">
-        <v>38</v>
+        <v>187</v>
       </c>
       <c r="B319" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="0" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="B320" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+      <c r="D320" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B321" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D321" s="0" t="s">
-        <v>202</v>
+        <v>10</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B322" s="0" t="s">
         <v>10</v>
@@ -3551,7 +3551,7 @@
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B323" s="0" t="s">
         <v>10</v>
@@ -3559,58 +3559,64 @@
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="0" t="s">
-        <v>206</v>
+        <v>15</v>
       </c>
       <c r="B324" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B325" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A326" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B326" s="0" t="s">
-        <v>12</v>
+    <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A327" s="0" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="0" t="s">
-        <v>207</v>
+        <v>1</v>
+      </c>
+      <c r="B328" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C328" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D328" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="0" t="s">
-        <v>1</v>
+        <v>208</v>
       </c>
       <c r="B329" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C329" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D329" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="0" t="s">
-        <v>208</v>
+        <v>22</v>
       </c>
       <c r="B330" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="C330" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D330" s="0" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B331" s="0" t="s">
         <v>8</v>
@@ -3622,23 +3628,17 @@
         <v>209</v>
       </c>
     </row>
-    <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B332" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C332" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D332" s="0" t="s">
-        <v>209</v>
+        <v>10</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="0" t="s">
-        <v>38</v>
+        <v>187</v>
       </c>
       <c r="B333" s="0" t="s">
         <v>10</v>
@@ -3646,71 +3646,63 @@
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="0" t="s">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="B334" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B335" s="0" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D335" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B336" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="D336" s="0" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B337" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B338" s="0" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>110</v>
+      </c>
+      <c r="D338" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="0" t="s">
-        <v>214</v>
+        <v>15</v>
       </c>
       <c r="B339" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="D339" s="0" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B340" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A341" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B341" s="0" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update README and table structure files to reflect recent changes
</commit_message>
<xml_diff>
--- a/table_structure.xlsx
+++ b/table_structure.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="214">
   <si>
     <t xml:space="preserve">baskets</t>
   </si>
@@ -367,13 +367,13 @@
     <t xml:space="preserve">BIGINT</t>
   </si>
   <si>
-    <t xml:space="preserve">ex_dividend</t>
+    <t xml:space="preserve">dividend</t>
   </si>
   <si>
     <t xml:space="preserve">DECIMAL(6,3)</t>
   </si>
   <si>
-    <t xml:space="preserve">split_ratio</t>
+    <t xml:space="preserve">split</t>
   </si>
   <si>
     <t xml:space="preserve">finra_data</t>
@@ -557,9 +557,6 @@
   </si>
   <si>
     <t xml:space="preserve">company</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dividend</t>
   </si>
   <si>
     <t xml:space="preserve">ex_dividend_date</t>
@@ -768,16 +765,16 @@
   </sheetPr>
   <dimension ref="A1:D340"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A87" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C124" activeCellId="0" sqref="C124"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A123" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A150" activeCellId="0" sqref="A150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.1902834008097"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.7935222672065"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.9068825910931"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.7044534412956"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.3643724696356"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.336032388664"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3139,7 +3136,7 @@
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="s">
-        <v>179</v>
+        <v>115</v>
       </c>
       <c r="B276" s="0" t="s">
         <v>116</v>
@@ -3147,7 +3144,7 @@
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="0" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B277" s="0" t="s">
         <v>109</v>
@@ -3158,7 +3155,7 @@
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B278" s="0" t="s">
         <v>12</v>
@@ -3166,7 +3163,7 @@
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B279" s="0" t="s">
         <v>12</v>
@@ -3174,7 +3171,7 @@
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B280" s="0" t="s">
         <v>12</v>
@@ -3198,7 +3195,7 @@
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3217,7 +3214,7 @@
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B286" s="0" t="s">
         <v>6</v>
@@ -3234,7 +3231,7 @@
         <v>23</v>
       </c>
       <c r="D287" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3248,7 +3245,7 @@
         <v>23</v>
       </c>
       <c r="D288" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3261,7 +3258,7 @@
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="0" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B290" s="0" t="s">
         <v>10</v>
@@ -3275,12 +3272,12 @@
         <v>109</v>
       </c>
       <c r="D291" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="0" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B292" s="0" t="s">
         <v>116</v>
@@ -3288,7 +3285,7 @@
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="0" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B293" s="0" t="s">
         <v>116</v>
@@ -3312,7 +3309,7 @@
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="0" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3331,7 +3328,7 @@
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="0" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B299" s="0" t="s">
         <v>6</v>
@@ -3348,7 +3345,7 @@
         <v>23</v>
       </c>
       <c r="D300" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3362,18 +3359,18 @@
         <v>23</v>
       </c>
       <c r="D301" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="0" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B302" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D302" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3384,12 +3381,12 @@
         <v>12</v>
       </c>
       <c r="D303" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="0" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B304" s="0" t="s">
         <v>12</v>
@@ -3397,7 +3394,7 @@
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="0" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B305" s="0" t="s">
         <v>10</v>
@@ -3405,7 +3402,7 @@
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="0" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B306" s="0" t="s">
         <v>10</v>
@@ -3413,7 +3410,7 @@
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="0" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B307" s="0" t="s">
         <v>10</v>
@@ -3421,7 +3418,7 @@
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="0" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B308" s="0" t="s">
         <v>10</v>
@@ -3429,7 +3426,7 @@
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="0" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B309" s="0" t="s">
         <v>10</v>
@@ -3453,7 +3450,7 @@
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="0" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3472,7 +3469,7 @@
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="0" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B315" s="0" t="s">
         <v>6</v>
@@ -3489,7 +3486,7 @@
         <v>23</v>
       </c>
       <c r="D316" s="0" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3503,7 +3500,7 @@
         <v>23</v>
       </c>
       <c r="D317" s="0" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3516,7 +3513,7 @@
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="0" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B319" s="0" t="s">
         <v>10</v>
@@ -3524,18 +3521,18 @@
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="0" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B320" s="0" t="s">
         <v>12</v>
       </c>
       <c r="D320" s="0" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="0" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B321" s="0" t="s">
         <v>10</v>
@@ -3543,7 +3540,7 @@
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="0" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B322" s="0" t="s">
         <v>10</v>
@@ -3551,7 +3548,7 @@
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="0" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B323" s="0" t="s">
         <v>10</v>
@@ -3575,7 +3572,7 @@
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="0" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3594,7 +3591,7 @@
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="0" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B329" s="0" t="s">
         <v>6</v>
@@ -3611,7 +3608,7 @@
         <v>23</v>
       </c>
       <c r="D330" s="0" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3625,7 +3622,7 @@
         <v>23</v>
       </c>
       <c r="D331" s="0" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3638,7 +3635,7 @@
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="0" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B333" s="0" t="s">
         <v>10</v>
@@ -3646,7 +3643,7 @@
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="0" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B334" s="0" t="s">
         <v>12</v>
@@ -3654,18 +3651,18 @@
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="0" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B335" s="0" t="s">
         <v>12</v>
       </c>
       <c r="D335" s="0" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="0" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B336" s="0" t="s">
         <v>12</v>
@@ -3673,7 +3670,7 @@
     </row>
     <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="0" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B337" s="0" t="s">
         <v>145</v>
@@ -3681,13 +3678,13 @@
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="0" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B338" s="0" t="s">
         <v>110</v>
       </c>
       <c r="D338" s="0" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>